<commit_message>
First cut at eta template.
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Allocation-sample.xlsx
+++ b/inst/extdata/GH-ZA-Allocation-sample.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Library/Containers/com.microsoft.Excel/Data/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FD3F0D-1D8A-AF48-9DF7-CF04088BD0AE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BECE6D-EC1B-6C4C-BC05-CE046953743B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Allocations" sheetId="1" r:id="rId1"/>
+    <sheet name="FU Allocations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>

</xml_diff>

<commit_message>
Working on eta template.
</commit_message>
<xml_diff>
--- a/inst/extdata/GH-ZA-Allocation-sample.xlsx
+++ b/inst/extdata/GH-ZA-Allocation-sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/IEATools/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BECE6D-EC1B-6C4C-BC05-CE046953743B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E7DE42-A679-B84D-88B9-6192B92283D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7278" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7279" uniqueCount="118">
   <si>
     <t>Country</t>
   </si>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O692"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A657" workbookViewId="0">
-      <selection activeCell="N690" sqref="N690:O691"/>
+    <sheetView tabSelected="1" topLeftCell="A667" workbookViewId="0">
+      <selection activeCell="J147" sqref="J147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3146,6 +3146,9 @@
       <c r="I59" t="s">
         <v>85</v>
       </c>
+      <c r="J59" t="s">
+        <v>81</v>
+      </c>
       <c r="K59" t="s">
         <v>44</v>
       </c>
@@ -5130,6 +5133,9 @@
       <c r="N109">
         <v>15</v>
       </c>
+      <c r="O109">
+        <v>15</v>
+      </c>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
@@ -5172,6 +5178,9 @@
       <c r="N110">
         <v>55</v>
       </c>
+      <c r="O110">
+        <v>55</v>
+      </c>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
@@ -5214,6 +5223,9 @@
       <c r="N111">
         <v>15</v>
       </c>
+      <c r="O111">
+        <v>15</v>
+      </c>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
@@ -5254,6 +5266,9 @@
       </c>
       <c r="M112" s="3"/>
       <c r="N112">
+        <v>15</v>
+      </c>
+      <c r="O112">
         <v>15</v>
       </c>
     </row>
@@ -6588,6 +6603,9 @@
       <c r="I146" t="s">
         <v>93</v>
       </c>
+      <c r="J146" t="s">
+        <v>112</v>
+      </c>
       <c r="K146" t="s">
         <v>51</v>
       </c>
@@ -15012,7 +15030,7 @@
         <v>55</v>
       </c>
       <c r="I360" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="J360" t="s">
         <v>79</v>
@@ -15054,12 +15072,6 @@
       <c r="H361" t="s">
         <v>55</v>
       </c>
-      <c r="I361" t="s">
-        <v>80</v>
-      </c>
-      <c r="J361" t="s">
-        <v>81</v>
-      </c>
       <c r="K361" t="s">
         <v>69</v>
       </c>
@@ -15225,7 +15237,7 @@
       <c r="M365" s="3"/>
       <c r="N365" s="3"/>
       <c r="O365">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="366" spans="1:15" x14ac:dyDescent="0.2">
@@ -15267,6 +15279,9 @@
       </c>
       <c r="M366" s="3"/>
       <c r="N366" s="3"/>
+      <c r="O366">
+        <v>50</v>
+      </c>
     </row>
     <row r="367" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
@@ -21153,6 +21168,9 @@
       <c r="I516" t="s">
         <v>91</v>
       </c>
+      <c r="J516" t="s">
+        <v>112</v>
+      </c>
       <c r="K516" t="s">
         <v>75</v>
       </c>
@@ -26037,6 +26055,9 @@
       </c>
       <c r="M640" s="3"/>
       <c r="N640" s="3"/>
+      <c r="O640">
+        <v>50</v>
+      </c>
     </row>
     <row r="641" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A641" t="s">
@@ -26077,6 +26098,9 @@
       </c>
       <c r="M641" s="3"/>
       <c r="N641" s="3"/>
+      <c r="O641">
+        <v>50</v>
+      </c>
     </row>
     <row r="642" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A642" t="s">

</xml_diff>